<commit_message>
Adding the same excel file as before with different type
</commit_message>
<xml_diff>
--- a/Survey_Results.xlsx
+++ b/Survey_Results.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Danial\1) Milan\1) University of Milan\4. First Trimester\4. Marketing\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Danial\1) Milan\1) University of Milan\4. First Trimester\4. Marketing\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A847684-902E-47EA-9179-A29E8DAF7051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77776688-FF3C-405A-B53D-C513AFDE51DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2EBAB415-A5F5-4FAF-9836-3E008D150698}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,6 +27,60 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="22">
   <si>
+    <t>respondent_id</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Preferred_1</t>
+  </si>
+  <si>
+    <t>Preferred_2</t>
+  </si>
+  <si>
+    <t>Preferred_3</t>
+  </si>
+  <si>
+    <t>Preferred_4</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Popularity of the place</t>
+  </si>
+  <si>
+    <t>Cultural/Historical activities</t>
+  </si>
+  <si>
+    <t>Social activities</t>
+  </si>
+  <si>
+    <t>Activities in nature</t>
+  </si>
+  <si>
+    <t>Gastronomical activities</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Discovery</t>
+  </si>
+  <si>
     <t>Friends</t>
   </si>
   <si>
@@ -46,77 +91,19 @@
   </si>
   <si>
     <t>Alone</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Velocity</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Discovery</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>Information</t>
-  </si>
-  <si>
-    <t>Popularity of the place</t>
-  </si>
-  <si>
-    <t>Cultural/Historical activities</t>
-  </si>
-  <si>
-    <t>Social activities</t>
-  </si>
-  <si>
-    <t>Activities in nature</t>
-  </si>
-  <si>
-    <t>Gastronomical activities</t>
-  </si>
-  <si>
-    <t>Weather</t>
-  </si>
-  <si>
-    <t>Preferred_1</t>
-  </si>
-  <si>
-    <t>Preferred_2</t>
-  </si>
-  <si>
-    <t>Preferred_3</t>
-  </si>
-  <si>
-    <t>Preferred_4</t>
-  </si>
-  <si>
-    <t>respondent_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Cambria"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,7 +162,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -187,7 +174,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -234,23 +221,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -286,23 +256,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,45 +407,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3577F71C-E492-4F93-93F7-16B08F303FAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
@@ -519,10 +469,10 @@
         <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -536,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -578,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -592,16 +542,16 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -634,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -648,16 +598,16 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -690,7 +640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -704,16 +654,16 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -746,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -760,16 +710,16 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -802,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -816,16 +766,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -858,7 +808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -872,16 +822,16 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -914,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -928,16 +878,16 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -970,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -984,16 +934,16 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1026,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1040,16 +990,16 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -1082,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1096,16 +1046,16 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -1138,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1152,16 +1102,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1194,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1208,16 +1158,16 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -1250,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1264,16 +1214,16 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I15">
         <v>3</v>
@@ -1306,7 +1256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1320,16 +1270,16 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1362,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1376,16 +1326,16 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1418,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1432,16 +1382,16 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -1474,7 +1424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1488,16 +1438,16 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I19">
         <v>5</v>
@@ -1530,7 +1480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1544,16 +1494,16 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="I20">
         <v>3</v>
@@ -1586,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1600,16 +1550,16 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1643,7 +1593,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the names of our features
</commit_message>
<xml_diff>
--- a/Survey_Results.xlsx
+++ b/Survey_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Danial\1) Milan\1) University of Milan\4. First Trimester\4. Marketing\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77776688-FF3C-405A-B53D-C513AFDE51DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA11080-1536-4E24-AB1D-E02D3DD108C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Velocity</t>
-  </si>
-  <si>
     <t>Preferred_1</t>
   </si>
   <si>
@@ -54,12 +51,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>Information</t>
-  </si>
-  <si>
     <t>Popularity of the place</t>
   </si>
   <si>
@@ -91,6 +82,15 @@
   </si>
   <si>
     <t>Alone</t>
+  </si>
+  <si>
+    <t>Travel Frequency</t>
+  </si>
+  <si>
+    <t>Accessibility of transportation</t>
+  </si>
+  <si>
+    <t>Availability of information</t>
   </si>
 </sst>
 </file>
@@ -411,10 +411,21 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R21"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -427,49 +438,49 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -486,16 +497,16 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -542,16 +553,16 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -598,16 +609,16 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -654,16 +665,16 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -710,16 +721,16 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -766,16 +777,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -822,16 +833,16 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -878,16 +889,16 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -934,16 +945,16 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -990,16 +1001,16 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -1046,16 +1057,16 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -1102,16 +1113,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1158,16 +1169,16 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -1214,16 +1225,16 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I15">
         <v>3</v>
@@ -1270,16 +1281,16 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1326,16 +1337,16 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1382,16 +1393,16 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -1438,16 +1449,16 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I19">
         <v>5</v>
@@ -1494,16 +1505,16 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I20">
         <v>3</v>
@@ -1550,16 +1561,16 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1594,5 +1605,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the jupyter file
</commit_message>
<xml_diff>
--- a/Survey_Results.xlsx
+++ b/Survey_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Danial\1) Milan\1) University of Milan\4. First Trimester\4. Marketing\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA11080-1536-4E24-AB1D-E02D3DD108C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632B8D94-D14B-434B-999B-72031D106896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>